<commit_message>
forest to share of land, 3 subset-weight
1) Changed variable of forest land cover from [ha] to share of land covered by forest; minimum and maximum taken from the regional AR6 database.
2) Implemented more sets of weights by: (i) partitioning the set of 6 indicators (with NOx and SOx counting as one) into 3 subsets (empty sets allowed); (ii) indicators in subsets receive the same weight; (iii) each subset receives a weight different than the others; (iv) weights of subset have a high, middle, and low value; (v) NOx and SOx receive the same weight.
Dataframes of indicators (same as before, only forest land cover changed) and welfare levels, saved to Rdata file.
</commit_message>
<xml_diff>
--- a/AR6_min_max_updates.xlsx
+++ b/AR6_min_max_updates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uk\Documents\GitHub\multidimwelfare-scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uk\Projects\Navigate\AlternativeWelfareMetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>AR6 climate diagnostics|Surface Temperature (GSAT)|MAGICCv7.5.3|50.0th Percentile</t>
   </si>
@@ -221,6 +221,15 @@
   </si>
   <si>
     <t>pre-industrial</t>
+  </si>
+  <si>
+    <t>Share land cover forest</t>
+  </si>
+  <si>
+    <t>share of land as forest</t>
+  </si>
+  <si>
+    <t>#adding share of forest in land cover</t>
   </si>
 </sst>
 </file>
@@ -439,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -474,6 +483,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -774,7 +784,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1431,6 +1441,42 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0.61</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15">
+        <f>E15</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>F15</f>
+        <v>0.61</v>
+      </c>
+    </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="T16" s="26"/>
     </row>

</xml_diff>